<commit_message>
add myFinanceManagerTest; log update;
</commit_message>
<xml_diff>
--- a/doc/log/log_201608040212_zouguo.xlsx
+++ b/doc/log/log_201608040212_zouguo.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19330"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2039A17-AA3B-494E-B06F-79F8F91F7037}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BEE53C7-AE8A-4DAA-A1D1-1185236443ED}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="36">
   <si>
     <t>周次</t>
   </si>
@@ -95,22 +95,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>第三天1:00-4:31</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>第四天1:00-4:32</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>第五天1:00-4:33</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>第七天1:00-4:35</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>学习Jenkins的使用以及相关知识</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -147,7 +131,31 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>第六天1:00-4:30</t>
+    <t>完善dao service 测试 以及完善代码注释</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>第三天1:00-4:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>第四天1:00-4:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>第五天1:00-4:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  第六天10:00-14:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 第七天9:00-17:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>第八天</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -537,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -732,7 +740,7 @@
         <v>17</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>2</v>
@@ -746,13 +754,13 @@
         <v>18</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
@@ -760,55 +768,55 @@
         <v>19</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="D16" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
@@ -816,15 +824,62 @@
         <v>33</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
-        <v>23</v>
+        <v>34</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A22" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A23" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A24" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A25" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A26" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A27" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A28" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>